<commit_message>
reporte general sin filtros
</commit_message>
<xml_diff>
--- a/public/reportes/ReporteGeneralEstudiantes.xlsx
+++ b/public/reportes/ReporteGeneralEstudiantes.xlsx
@@ -1,25 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leluc\Documents\Proyectos\SICA\Back\Api_SICA\public\reportes\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
-  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
   <si>
     <t>REPORTE GENERAL DE ESTUDIANTES</t>
   </si>
@@ -39,53 +32,311 @@
     <t>HORARIO SALIDA</t>
   </si>
   <si>
-    <t>FECHA DE ASISTENCIA</t>
+    <t>FECHA DE ASISTENCIA (ENTRADA)</t>
   </si>
   <si>
     <t>HORA DE ENTRADA</t>
   </si>
   <si>
+    <t>FECHA DE ASISTENCIA (SALIDA)</t>
+  </si>
+  <si>
     <t>HORA DE SALIDA</t>
   </si>
   <si>
     <t>TOTAL DE HORAS</t>
+  </si>
+  <si>
+    <t>Yanick Gerardo Rodríguez Hernández</t>
+  </si>
+  <si>
+    <t>Carmina Arellano Fernández</t>
+  </si>
+  <si>
+    <t>13:00:00</t>
+  </si>
+  <si>
+    <t>17:00:00</t>
+  </si>
+  <si>
+    <t>Irwin Alfonso Gamez Gándara</t>
+  </si>
+  <si>
+    <t>Dora María Rodríguez Martínez</t>
+  </si>
+  <si>
+    <t>09:00:00</t>
+  </si>
+  <si>
+    <t>Emma Rodríguez Tovar</t>
+  </si>
+  <si>
+    <t>Arturo Gonzalo Rivera García</t>
+  </si>
+  <si>
+    <t>08:00:00</t>
+  </si>
+  <si>
+    <t>12:00:00</t>
+  </si>
+  <si>
+    <t>Samantha Monserrat Reyes Calva</t>
+  </si>
+  <si>
+    <t>María Guadalupe Rodríguez Serrato</t>
+  </si>
+  <si>
+    <t>Fabrizio Villafuerte Nájera</t>
+  </si>
+  <si>
+    <t>Jesús Emiliano Briones Esquivel</t>
+  </si>
+  <si>
+    <t>Carlos Javier Garza Leal</t>
+  </si>
+  <si>
+    <t>Perla Cecilia Cortés Dávila</t>
+  </si>
+  <si>
+    <t>Verónica Alejandra Regalado Gonzalez</t>
+  </si>
+  <si>
+    <t>José Francisco Navarro Medrano</t>
+  </si>
+  <si>
+    <t>Iván Znitch Villarreal López</t>
+  </si>
+  <si>
+    <t>Gerardo Guadalupe Uvalle Callente</t>
+  </si>
+  <si>
+    <t>Pedro Higinio Salazar Obregon</t>
+  </si>
+  <si>
+    <t>Juan Emmanuel Pérez Morales</t>
+  </si>
+  <si>
+    <t>Jonathan Omsare López Nieto</t>
+  </si>
+  <si>
+    <t>14:00:00</t>
+  </si>
+  <si>
+    <t>18:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Omri Omar Durán Porras</t>
+  </si>
+  <si>
+    <t>Daphne Carolina Salinas Juárez</t>
+  </si>
+  <si>
+    <t>Diana Dávalos Guerra</t>
+  </si>
+  <si>
+    <t>Victoria Rubí Banda Rodríguez</t>
+  </si>
+  <si>
+    <t>Diego Alonso Aguilar Reyna</t>
+  </si>
+  <si>
+    <t>11:30:00</t>
+  </si>
+  <si>
+    <t>15:30:00</t>
+  </si>
+  <si>
+    <t>Jesús Alberto Díaz Zúñiga</t>
+  </si>
+  <si>
+    <t>Andriy Raphael Flores Sigala</t>
+  </si>
+  <si>
+    <t>Adriana Espinosa Rodríguez</t>
+  </si>
+  <si>
+    <t>Paloma Monserrat Escamilla García</t>
+  </si>
+  <si>
+    <t>Jorge Omar Del Valle Díaz</t>
+  </si>
+  <si>
+    <t>15:00:00</t>
+  </si>
+  <si>
+    <t>19:00:00</t>
+  </si>
+  <si>
+    <t>Gabriel Rodríguez de la Fuente</t>
+  </si>
+  <si>
+    <t>Israel Yasim Martinez Camacho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yamileth Pesina Martínez </t>
+  </si>
+  <si>
+    <t>Victoria Guadalupe Ortega Pérez</t>
+  </si>
+  <si>
+    <t>Daniela Alejandra Marquina López</t>
+  </si>
+  <si>
+    <t>Héctor Enrique Ibarra Ibarra</t>
+  </si>
+  <si>
+    <t>Mónica Cristina Jáuregui Moreno</t>
+  </si>
+  <si>
+    <t>María Idalia Arroyo Rodriguez</t>
+  </si>
+  <si>
+    <t>Fabiola Martínez Marín</t>
+  </si>
+  <si>
+    <t>Jorge Omar del Valle Díaz</t>
+  </si>
+  <si>
+    <t>11:00:00</t>
+  </si>
+  <si>
+    <t>Cuauhtémoc Cardona Arciniega</t>
+  </si>
+  <si>
+    <t>16:00:00</t>
+  </si>
+  <si>
+    <t>Yareli Viridiana Eguía Bazaldúa</t>
+  </si>
+  <si>
+    <t>Rosalba Aguilar Diaz</t>
+  </si>
+  <si>
+    <t>Estefany Lugo Lara</t>
+  </si>
+  <si>
+    <t>Francisco Javier Aguayo Inés</t>
+  </si>
+  <si>
+    <t>Mónica Valeria Garay Muñoz</t>
+  </si>
+  <si>
+    <t>Alicia Guadalupe Torres Garza</t>
+  </si>
+  <si>
+    <t>Carolina Iveth Trejo Reyna</t>
+  </si>
+  <si>
+    <t>Miranda Giselle Espinoza Alvarado</t>
+  </si>
+  <si>
+    <t>Susana Patricia Servín Palacios</t>
+  </si>
+  <si>
+    <t>Alma Edith Reynoso Najera</t>
+  </si>
+  <si>
+    <t>Javier Alejandro Carrizales Ávalos</t>
+  </si>
+  <si>
+    <t>Jessica Itzel Espinoza Lopez</t>
+  </si>
+  <si>
+    <t>Melanie Guadalupe Bernal Ibarra</t>
+  </si>
+  <si>
+    <t>Lourie Dafne Pérez Cruz</t>
+  </si>
+  <si>
+    <t>Roberto Carlos Gallegos García</t>
+  </si>
+  <si>
+    <t>Mario Antonio Tovar Herrera</t>
+  </si>
+  <si>
+    <t>Carlos Cuéllar Galván</t>
+  </si>
+  <si>
+    <t>Rocio Esmeralda Martinez Lucio</t>
+  </si>
+  <si>
+    <t>Ana Rebeca Esparza Alvarado</t>
+  </si>
+  <si>
+    <t>David Israel Ledezma Martínez</t>
+  </si>
+  <si>
+    <t>Valeria Arleth Martínez Beltrán</t>
+  </si>
+  <si>
+    <t>Jaci Jeanhine Ruiz Erazo</t>
+  </si>
+  <si>
+    <t>Yvonne Xiomara Casas Gallegos</t>
+  </si>
+  <si>
+    <t>Ana Lucía Rico Gomez</t>
+  </si>
+  <si>
+    <t>Claudia Nallely Puente Obregón</t>
+  </si>
+  <si>
+    <t>Jonathan Eduardo Martínez Saldaña</t>
+  </si>
+  <si>
+    <t>Lina Rebeca Moya Bautista</t>
+  </si>
+  <si>
+    <t>Shellzy Alicia Reyes Reyes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kenia Alejandra González Cavazos </t>
+  </si>
+  <si>
+    <t>Mariana Guadalupe Barrios Araujo</t>
+  </si>
+  <si>
+    <t>Glenis Beatriz Giménez Hidalgo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,12 +353,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -137,36 +382,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -490,22 +727,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="B1">
+      <selection activeCell="A1" sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="8.7265625" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="27.1796875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="59.81640625" customWidth="1"/>
-    <col min="3" max="3" width="23.90625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" customWidth="1"/>
+    <col min="1" max="1" width="27.1796875" customWidth="true" style="3"/>
+    <col min="2" max="2" width="59.81640625" customWidth="true" style="0"/>
+    <col min="3" max="3" width="23.90625" customWidth="true" style="3"/>
+    <col min="6" max="6" width="10.90625" customWidth="true" style="0"/>
+    <col min="7" max="7" width="10.90625" customWidth="true" style="0"/>
+    <col min="8" max="8" width="10.90625" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -517,8 +759,9 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
-    </row>
-    <row r="2" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" customHeight="1" ht="43.5">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -546,12 +789,1117 @@
       <c r="I2" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="J2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" t="s">
+        <v>63</v>
+      </c>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" t="s">
+        <v>63</v>
+      </c>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D48" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" t="s">
+        <v>14</v>
+      </c>
+      <c r="F49"/>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50" t="s">
+        <v>35</v>
+      </c>
+      <c r="E50" t="s">
+        <v>36</v>
+      </c>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51"/>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+      <c r="J51">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D52" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52"/>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+      <c r="J52">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D53" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53"/>
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="I53"/>
+      <c r="J53">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D54" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54"/>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54"/>
+      <c r="J54">
+        <v>0.0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+  <mergeCells>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="1" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" r:id="rId1ps"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>